<commit_message>
Commit on 08 Apr 2023
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMparamTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMparamTestData.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="60" windowWidth="27795" windowHeight="12090" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="27795" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="CSMParam_GeneralLedgerTestData" sheetId="1" r:id="rId1"/>
     <sheet name="CSMParam_AccountTypeTestData" sheetId="2" r:id="rId2"/>
     <sheet name="CSMParam_userAccessTestData" sheetId="3" r:id="rId3"/>
+    <sheet name="CSMParam_CIFTypeTestData" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -156,14 +157,40 @@
     <t>DS01_ActType_Acces_04</t>
   </si>
   <si>
-    <t>9637</t>
+    <t>CIF Type Code</t>
+  </si>
+  <si>
+    <t>CIF Type</t>
+  </si>
+  <si>
+    <t>Economic Sector</t>
+  </si>
+  <si>
+    <t>Sub Economic Sector</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Legal Status</t>
+  </si>
+  <si>
+    <t>Allow Gl Code</t>
+  </si>
+  <si>
+    <t>CIFType_01</t>
+  </si>
+  <si>
+    <t>DS_01_CIFType_01</t>
+  </si>
+  <si>
+    <t>Individual</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -211,7 +238,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -234,19 +261,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -543,19 +586,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="5.62109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="16.42578125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="21.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="26.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -588,8 +631,8 @@
       <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>46</v>
+      <c r="C2" s="3">
+        <v>9642</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>9</v>
@@ -612,7 +655,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="3">
-        <v>9626</v>
+        <v>9643</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>9</v>
@@ -635,7 +678,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="3">
-        <v>9627</v>
+        <v>9644</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>9</v>
@@ -658,7 +701,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="3">
-        <v>9628</v>
+        <v>9645</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>9</v>
@@ -683,18 +726,18 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="28.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.4375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="30.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="29.140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="1" max="1" width="28.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29" customWidth="1"/>
+    <col min="4" max="4" width="30.85546875" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -724,9 +767,7 @@
       <c r="B2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>46</v>
-      </c>
+      <c r="C2" s="5"/>
       <c r="D2" s="3" t="s">
         <v>26</v>
       </c>
@@ -783,19 +824,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="28.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="12.69921875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="39.5703125" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="39.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -831,14 +872,14 @@
       <c r="C2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="6" t="s">
+      <c r="D2" s="6">
+        <v>9636</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="8" t="s">
         <v>44</v>
       </c>
     </row>
@@ -852,15 +893,113 @@
       <c r="C3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6">
+        <v>9636</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
+    <col min="9" max="9" width="30" customWidth="1"/>
+    <col min="10" max="10" width="22.85546875" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="7"/>
-      <c r="F3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>44</v>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="10">
+        <v>9611</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="10">
+        <v>1</v>
+      </c>
+      <c r="H2" s="10">
+        <v>1</v>
+      </c>
+      <c r="I2" s="10">
+        <v>62</v>
+      </c>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" s="6">
+        <v>9601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cheuqebook request pending test case commit
</commit_message>
<xml_diff>
--- a/AzentioAutomationFramework_CSMAnandh/TestData/CSMparamTestData.xlsx
+++ b/AzentioAutomationFramework_CSMAnandh/TestData/CSMparamTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="14940" windowHeight="9225" tabRatio="1000" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="CSMParam_GeneralLedgerTestData" sheetId="1" r:id="rId1"/>
@@ -13,13 +13,15 @@
     <sheet name="CSMParam_CIFTypeTestData" sheetId="4" r:id="rId4"/>
     <sheet name="CSMParam_TransactionTypeTestDat" sheetId="5" r:id="rId5"/>
     <sheet name="ChargeCodeTestData" sheetId="6" r:id="rId6"/>
+    <sheet name="Cheques_ChequeBookTestData" sheetId="7" r:id="rId7"/>
+    <sheet name="CSMParam_ControlRecordsTestData" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="210">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -590,6 +592,156 @@
   <si>
     <t>DS01_CW_039_02</t>
   </si>
+  <si>
+    <t>Chequebook code</t>
+  </si>
+  <si>
+    <t>Gl Code</t>
+  </si>
+  <si>
+    <t>CHB_055_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_055_01</t>
+  </si>
+  <si>
+    <t>Update dataset ID 1</t>
+  </si>
+  <si>
+    <t>DS01_CHB_055</t>
+  </si>
+  <si>
+    <t>CHB_057_01</t>
+  </si>
+  <si>
+    <t>CHB_058_01</t>
+  </si>
+  <si>
+    <t>CHB_059_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_057_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_058_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_059_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_057</t>
+  </si>
+  <si>
+    <t>DS01_CHB_058</t>
+  </si>
+  <si>
+    <t>DS01_CHB_059</t>
+  </si>
+  <si>
+    <t>CHB_060_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_060_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_060</t>
+  </si>
+  <si>
+    <t>CHB_062_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_062_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_062</t>
+  </si>
+  <si>
+    <t>CHB_063_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_063_01</t>
+  </si>
+  <si>
+    <t>CHB_064_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_064_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_064</t>
+  </si>
+  <si>
+    <t>DS01_CHB_063</t>
+  </si>
+  <si>
+    <t>CHB_067_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_067_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_067</t>
+  </si>
+  <si>
+    <t>CHB_065_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_065_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_065</t>
+  </si>
+  <si>
+    <t>CHB_066_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_066_01</t>
+  </si>
+  <si>
+    <t>CHB_081_02</t>
+  </si>
+  <si>
+    <t>DS01_CHB_081_02</t>
+  </si>
+  <si>
+    <t>Cheque Unique Based On</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>CHB_081_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_081_01</t>
+  </si>
+  <si>
+    <t>Update dataset ID 2</t>
+  </si>
+  <si>
+    <t>DS01_CHB_081</t>
+  </si>
+  <si>
+    <t>DS01_CHB_082</t>
+  </si>
+  <si>
+    <t>CHB_074_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_074_01</t>
+  </si>
+  <si>
+    <t>DS01_CHB_074</t>
+  </si>
+  <si>
+    <t>CHB_075_02</t>
+  </si>
+  <si>
+    <t>DS01_CHB_075_01</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
 </sst>
 </file>
 
@@ -598,7 +750,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -664,6 +816,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF363636"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -825,7 +983,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -866,6 +1024,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Excel_20_Built-in_20_Normal" xfId="5"/>
@@ -1183,7 +1347,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2519,8 +2683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2588,4 +2752,380 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:XFD13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" customWidth="1"/>
+    <col min="6" max="6" width="26.85546875" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="32" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>161</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>164</v>
+      </c>
+      <c r="G1" s="43" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="C2" s="40">
+        <v>7689</v>
+      </c>
+      <c r="D2" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E2" s="40">
+        <v>840</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="20"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="40">
+        <v>7689</v>
+      </c>
+      <c r="D3" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E3" s="40">
+        <v>840</v>
+      </c>
+      <c r="F3" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" s="20"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="C4" s="40">
+        <v>7689</v>
+      </c>
+      <c r="D4" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E4" s="40">
+        <v>840</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="G4" s="20"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C5" s="40">
+        <v>7689</v>
+      </c>
+      <c r="D5" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E5" s="40">
+        <v>840</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="G5" s="20"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="40">
+        <v>7689</v>
+      </c>
+      <c r="D6" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E6" s="40">
+        <v>840</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="G6" s="20"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="C7" s="40">
+        <v>888</v>
+      </c>
+      <c r="D7" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E7" s="40">
+        <v>840</v>
+      </c>
+      <c r="F7" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G7" s="20"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="20" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="40">
+        <v>888</v>
+      </c>
+      <c r="D8" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E8" s="40">
+        <v>840</v>
+      </c>
+      <c r="F8" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="G8" s="20"/>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="C9" s="40">
+        <v>888</v>
+      </c>
+      <c r="D9" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E9" s="40">
+        <v>840</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>185</v>
+      </c>
+      <c r="G9" s="20"/>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="40">
+        <v>888</v>
+      </c>
+      <c r="D10" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E10" s="40">
+        <v>840</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="20" t="s">
+        <v>193</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="40">
+        <v>888</v>
+      </c>
+      <c r="D11" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E11" s="40">
+        <v>840</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="20" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="C12" s="40">
+        <v>888</v>
+      </c>
+      <c r="D12" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E12" s="40">
+        <v>840</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>189</v>
+      </c>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="20" t="s">
+        <v>204</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="40">
+        <v>888</v>
+      </c>
+      <c r="D13" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E13" s="40">
+        <v>840</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>206</v>
+      </c>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="20" t="s">
+        <v>199</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" s="40">
+        <v>888</v>
+      </c>
+      <c r="D14" s="41">
+        <v>96137</v>
+      </c>
+      <c r="E14" s="40">
+        <v>840</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>202</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>203</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15">
+      <c r="A1" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="20" t="s">
+        <v>195</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="42" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>